<commit_message>
Doc: Updated CIL file with new Items
</commit_message>
<xml_diff>
--- a/Project Management Plan/CIL.xlsx
+++ b/Project Management Plan/CIL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Project Management Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BD3D6F-5C6F-43FA-A46C-64A5E12646C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC20D86-4392-42A5-B2BE-680424B85986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Item</t>
   </si>
@@ -107,13 +107,31 @@
   </si>
   <si>
     <t>Requirments/SRS.xlsx</t>
+  </si>
+  <si>
+    <t>Test-Cases</t>
+  </si>
+  <si>
+    <t>Test/Test-cases.xlsx</t>
+  </si>
+  <si>
+    <t>https://github.com/abdallahEl-Karamany/Online-Mobile-Store-WebSite/blob/fa2db1bd6489d333e0da55760b2e98aa852b2bc2/Test/Test-cases.xlsx</t>
+  </si>
+  <si>
+    <t>WireFrames</t>
+  </si>
+  <si>
+    <t>WireFrame</t>
+  </si>
+  <si>
+    <t>https://github.com/abdallahEl-Karamany/Online-Mobile-Store-WebSite/tree/fa2db1bd6489d333e0da55760b2e98aa852b2bc2/WireFrame</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -158,6 +176,13 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -237,37 +262,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,7 +515,7 @@
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:H14"/>
+      <selection activeCell="B16" sqref="B16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -498,65 +526,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="3" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="7"/>
@@ -565,17 +593,17 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="7"/>
@@ -584,17 +612,17 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="13" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="7"/>
@@ -603,17 +631,17 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="7"/>
@@ -622,17 +650,17 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="13" t="s">
         <v>19</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="7"/>
@@ -641,17 +669,17 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="7"/>
@@ -660,17 +688,17 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="13" t="s">
         <v>25</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="7"/>
@@ -679,40 +707,52 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="13" t="s">
         <v>28</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
+      <c r="A13" s="2"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -725,7 +765,7 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
+      <c r="A14" s="2"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -738,7 +778,7 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
+      <c r="A15" s="2"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -751,7 +791,7 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
+      <c r="A16" s="2"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -764,7 +804,7 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
+      <c r="A17" s="2"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -777,7 +817,7 @@
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="2"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -790,7 +830,7 @@
       <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -803,7 +843,7 @@
       <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+      <c r="A20" s="2"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -816,7 +856,7 @@
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
+      <c r="A21" s="2"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -829,7 +869,7 @@
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -842,7 +882,7 @@
       <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
+      <c r="A23" s="2"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -855,7 +895,7 @@
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
+      <c r="A24" s="2"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -868,7 +908,7 @@
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
+      <c r="A25" s="2"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -881,7 +921,7 @@
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
+      <c r="A26" s="2"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -894,7 +934,7 @@
       <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
+      <c r="A27" s="2"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -907,7 +947,7 @@
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
+      <c r="A28" s="2"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -920,7 +960,7 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
+      <c r="A29" s="2"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -933,7 +973,7 @@
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
+      <c r="A30" s="2"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -946,7 +986,7 @@
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
+      <c r="A31" s="2"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -959,7 +999,7 @@
       <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
+      <c r="A32" s="2"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -972,7 +1012,7 @@
       <c r="K32" s="7"/>
     </row>
     <row r="33" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
+      <c r="A33" s="2"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -985,7 +1025,7 @@
       <c r="K33" s="7"/>
     </row>
     <row r="34" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
+      <c r="A34" s="2"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -998,7 +1038,7 @@
       <c r="K34" s="7"/>
     </row>
     <row r="35" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
+      <c r="A35" s="2"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1011,7 +1051,7 @@
       <c r="K35" s="7"/>
     </row>
     <row r="36" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
+      <c r="A36" s="2"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1024,7 +1064,7 @@
       <c r="K36" s="7"/>
     </row>
     <row r="37" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
+      <c r="A37" s="2"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1037,7 +1077,7 @@
       <c r="K37" s="7"/>
     </row>
     <row r="38" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
+      <c r="A38" s="2"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1050,7 +1090,7 @@
       <c r="K38" s="7"/>
     </row>
     <row r="39" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
+      <c r="A39" s="2"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1063,7 +1103,7 @@
       <c r="K39" s="7"/>
     </row>
     <row r="40" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
+      <c r="A40" s="2"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -1076,7 +1116,7 @@
       <c r="K40" s="7"/>
     </row>
     <row r="41" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -1089,7 +1129,7 @@
       <c r="K41" s="7"/>
     </row>
     <row r="42" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -1102,7 +1142,7 @@
       <c r="K42" s="7"/>
     </row>
     <row r="43" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
+      <c r="A43" s="2"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -1115,7 +1155,7 @@
       <c r="K43" s="7"/>
     </row>
     <row r="44" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
+      <c r="A44" s="2"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -1128,7 +1168,7 @@
       <c r="K44" s="7"/>
     </row>
     <row r="45" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
+      <c r="A45" s="2"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -1141,7 +1181,7 @@
       <c r="K45" s="7"/>
     </row>
     <row r="46" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="5"/>
+      <c r="A46" s="2"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -1154,7 +1194,7 @@
       <c r="K46" s="7"/>
     </row>
     <row r="47" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="5"/>
+      <c r="A47" s="2"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -1167,7 +1207,7 @@
       <c r="K47" s="7"/>
     </row>
     <row r="48" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
+      <c r="A48" s="2"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -1180,7 +1220,7 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
+      <c r="A49" s="2"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -1193,7 +1233,7 @@
       <c r="K49" s="7"/>
     </row>
     <row r="50" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="5"/>
+      <c r="A50" s="2"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -1206,7 +1246,7 @@
       <c r="K50" s="7"/>
     </row>
     <row r="51" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="5"/>
+      <c r="A51" s="2"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
@@ -1219,7 +1259,7 @@
       <c r="K51" s="7"/>
     </row>
     <row r="52" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
+      <c r="A52" s="2"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
@@ -1232,7 +1272,7 @@
       <c r="K52" s="7"/>
     </row>
     <row r="53" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="5"/>
+      <c r="A53" s="2"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
@@ -1245,7 +1285,7 @@
       <c r="K53" s="7"/>
     </row>
     <row r="54" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A54" s="5"/>
+      <c r="A54" s="2"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
@@ -1258,7 +1298,7 @@
       <c r="K54" s="7"/>
     </row>
     <row r="55" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="12"/>
+      <c r="A55" s="5"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -1271,7 +1311,7 @@
       <c r="K55" s="7"/>
     </row>
     <row r="56" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="12"/>
+      <c r="A56" s="5"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -1284,7 +1324,7 @@
       <c r="K56" s="7"/>
     </row>
     <row r="57" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="12"/>
+      <c r="A57" s="5"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -1297,7 +1337,7 @@
       <c r="K57" s="7"/>
     </row>
     <row r="58" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="13"/>
+      <c r="A58" s="6"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -1310,7 +1350,7 @@
       <c r="K58" s="7"/>
     </row>
     <row r="59" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="13"/>
+      <c r="A59" s="6"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -1323,7 +1363,7 @@
       <c r="K59" s="7"/>
     </row>
     <row r="60" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="13"/>
+      <c r="A60" s="6"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -1336,7 +1376,7 @@
       <c r="K60" s="7"/>
     </row>
     <row r="61" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="13"/>
+      <c r="A61" s="6"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
@@ -1349,7 +1389,7 @@
       <c r="K61" s="7"/>
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="9"/>
+      <c r="A62" s="4"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -1362,7 +1402,7 @@
       <c r="K62" s="7"/>
     </row>
     <row r="63" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="9"/>
+      <c r="A63" s="4"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -1375,7 +1415,7 @@
       <c r="K63" s="7"/>
     </row>
     <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="9"/>
+      <c r="A64" s="4"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -1388,7 +1428,7 @@
       <c r="K64" s="7"/>
     </row>
     <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="9"/>
+      <c r="A65" s="4"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -1401,7 +1441,7 @@
       <c r="K65" s="7"/>
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="9"/>
+      <c r="A66" s="4"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -1414,7 +1454,7 @@
       <c r="K66" s="7"/>
     </row>
     <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="9"/>
+      <c r="A67" s="4"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
@@ -1427,7 +1467,7 @@
       <c r="K67" s="7"/>
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="9"/>
+      <c r="A68" s="4"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -1440,7 +1480,7 @@
       <c r="K68" s="7"/>
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="9"/>
+      <c r="A69" s="4"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
@@ -1453,7 +1493,7 @@
       <c r="K69" s="7"/>
     </row>
     <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="9"/>
+      <c r="A70" s="4"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -1466,7 +1506,7 @@
       <c r="K70" s="7"/>
     </row>
     <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="9"/>
+      <c r="A71" s="4"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -1479,7 +1519,7 @@
       <c r="K71" s="7"/>
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="9"/>
+      <c r="A72" s="4"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -1492,7 +1532,7 @@
       <c r="K72" s="7"/>
     </row>
     <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="9"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -1505,7 +1545,7 @@
       <c r="K73" s="7"/>
     </row>
     <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="9"/>
+      <c r="A74" s="4"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -1518,7 +1558,7 @@
       <c r="K74" s="7"/>
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="9"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -1531,7 +1571,7 @@
       <c r="K75" s="7"/>
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="9"/>
+      <c r="A76" s="4"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -1544,7 +1584,7 @@
       <c r="K76" s="7"/>
     </row>
     <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="9"/>
+      <c r="A77" s="4"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -1557,7 +1597,7 @@
       <c r="K77" s="7"/>
     </row>
     <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="9"/>
+      <c r="A78" s="4"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -1570,223 +1610,389 @@
       <c r="K78" s="7"/>
     </row>
     <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
     </row>
     <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
     </row>
     <row r="81" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
     </row>
     <row r="82" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1"/>
-      <c r="K82" s="1"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
     </row>
     <row r="83" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
     </row>
     <row r="84" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
-      <c r="J84" s="1"/>
-      <c r="K84" s="1"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
     </row>
     <row r="85" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-      <c r="K85" s="1"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
     </row>
     <row r="86" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
     </row>
     <row r="87" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
     </row>
     <row r="88" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-      <c r="K88" s="1"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="14"/>
     </row>
     <row r="89" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="1"/>
-      <c r="J89" s="1"/>
-      <c r="K89" s="1"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
     </row>
     <row r="90" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
     </row>
     <row r="91" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-      <c r="K91" s="1"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
     </row>
     <row r="92" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
     </row>
     <row r="93" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-      <c r="K93" s="1"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+      <c r="K93" s="14"/>
     </row>
     <row r="94" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="1"/>
-      <c r="J94" s="1"/>
-      <c r="K94" s="1"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="14"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="14"/>
+      <c r="K94" s="14"/>
     </row>
     <row r="95" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-      <c r="K95" s="1"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="14"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="14"/>
     </row>
     <row r="96" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
-      <c r="J96" s="1"/>
-      <c r="K96" s="1"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="14"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
+      <c r="K96" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="190">
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="B54:H54"/>
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="B64:H64"/>
+    <mergeCell ref="B65:H65"/>
+    <mergeCell ref="B66:H66"/>
+    <mergeCell ref="B67:H67"/>
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="B71:H71"/>
+    <mergeCell ref="B72:H72"/>
+    <mergeCell ref="B73:H73"/>
+    <mergeCell ref="B74:H74"/>
+    <mergeCell ref="B75:H75"/>
+    <mergeCell ref="B76:H76"/>
+    <mergeCell ref="B77:H77"/>
+    <mergeCell ref="B78:H78"/>
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="B81:H81"/>
+    <mergeCell ref="B82:H82"/>
+    <mergeCell ref="B83:H83"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="B86:H86"/>
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="B95:H95"/>
+    <mergeCell ref="B96:H96"/>
+    <mergeCell ref="B88:H88"/>
+    <mergeCell ref="B89:H89"/>
+    <mergeCell ref="B90:H90"/>
+    <mergeCell ref="B91:H91"/>
+    <mergeCell ref="B92:H92"/>
+    <mergeCell ref="B93:H93"/>
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="I60:K60"/>
+    <mergeCell ref="I61:K61"/>
+    <mergeCell ref="I62:K62"/>
+    <mergeCell ref="I63:K63"/>
+    <mergeCell ref="I64:K64"/>
+    <mergeCell ref="I65:K65"/>
+    <mergeCell ref="I66:K66"/>
+    <mergeCell ref="I67:K67"/>
+    <mergeCell ref="I68:K68"/>
+    <mergeCell ref="I69:K69"/>
+    <mergeCell ref="I70:K70"/>
+    <mergeCell ref="I71:K71"/>
+    <mergeCell ref="I72:K72"/>
+    <mergeCell ref="I73:K73"/>
+    <mergeCell ref="I74:K74"/>
+    <mergeCell ref="I75:K75"/>
+    <mergeCell ref="I76:K76"/>
+    <mergeCell ref="I77:K77"/>
+    <mergeCell ref="I78:K78"/>
+    <mergeCell ref="I79:K79"/>
+    <mergeCell ref="I80:K80"/>
+    <mergeCell ref="I81:K81"/>
+    <mergeCell ref="I82:K82"/>
+    <mergeCell ref="I83:K83"/>
+    <mergeCell ref="I84:K84"/>
+    <mergeCell ref="I85:K85"/>
+    <mergeCell ref="I86:K86"/>
+    <mergeCell ref="I94:K94"/>
+    <mergeCell ref="I95:K95"/>
+    <mergeCell ref="I96:K96"/>
+    <mergeCell ref="I87:K87"/>
+    <mergeCell ref="I88:K88"/>
+    <mergeCell ref="I89:K89"/>
+    <mergeCell ref="I90:K90"/>
+    <mergeCell ref="I91:K91"/>
+    <mergeCell ref="I92:K92"/>
+    <mergeCell ref="I93:K93"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
     <mergeCell ref="I47:K47"/>
     <mergeCell ref="I48:K48"/>
     <mergeCell ref="I49:K49"/>
@@ -1811,172 +2017,6 @@
     <mergeCell ref="I35:K35"/>
     <mergeCell ref="I36:K36"/>
     <mergeCell ref="I37:K37"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I95:K95"/>
-    <mergeCell ref="I96:K96"/>
-    <mergeCell ref="I87:K87"/>
-    <mergeCell ref="I88:K88"/>
-    <mergeCell ref="I89:K89"/>
-    <mergeCell ref="I90:K90"/>
-    <mergeCell ref="I91:K91"/>
-    <mergeCell ref="I92:K92"/>
-    <mergeCell ref="I93:K93"/>
-    <mergeCell ref="I79:K79"/>
-    <mergeCell ref="I80:K80"/>
-    <mergeCell ref="I81:K81"/>
-    <mergeCell ref="I82:K82"/>
-    <mergeCell ref="I83:K83"/>
-    <mergeCell ref="I84:K84"/>
-    <mergeCell ref="I85:K85"/>
-    <mergeCell ref="I86:K86"/>
-    <mergeCell ref="I94:K94"/>
-    <mergeCell ref="I70:K70"/>
-    <mergeCell ref="I71:K71"/>
-    <mergeCell ref="I72:K72"/>
-    <mergeCell ref="I73:K73"/>
-    <mergeCell ref="I74:K74"/>
-    <mergeCell ref="I75:K75"/>
-    <mergeCell ref="I76:K76"/>
-    <mergeCell ref="I77:K77"/>
-    <mergeCell ref="I78:K78"/>
-    <mergeCell ref="I61:K61"/>
-    <mergeCell ref="I62:K62"/>
-    <mergeCell ref="I63:K63"/>
-    <mergeCell ref="I64:K64"/>
-    <mergeCell ref="I65:K65"/>
-    <mergeCell ref="I66:K66"/>
-    <mergeCell ref="I67:K67"/>
-    <mergeCell ref="I68:K68"/>
-    <mergeCell ref="I69:K69"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="I57:K57"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="I59:K59"/>
-    <mergeCell ref="I60:K60"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="B50:H50"/>
-    <mergeCell ref="B51:H51"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B96:H96"/>
-    <mergeCell ref="B88:H88"/>
-    <mergeCell ref="B89:H89"/>
-    <mergeCell ref="B90:H90"/>
-    <mergeCell ref="B91:H91"/>
-    <mergeCell ref="B92:H92"/>
-    <mergeCell ref="B93:H93"/>
-    <mergeCell ref="B94:H94"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="B81:H81"/>
-    <mergeCell ref="B82:H82"/>
-    <mergeCell ref="B83:H83"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B85:H85"/>
-    <mergeCell ref="B86:H86"/>
-    <mergeCell ref="B87:H87"/>
-    <mergeCell ref="B95:H95"/>
-    <mergeCell ref="B71:H71"/>
-    <mergeCell ref="B72:H72"/>
-    <mergeCell ref="B73:H73"/>
-    <mergeCell ref="B74:H74"/>
-    <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B76:H76"/>
-    <mergeCell ref="B77:H77"/>
-    <mergeCell ref="B78:H78"/>
-    <mergeCell ref="B79:H79"/>
-    <mergeCell ref="B62:H62"/>
-    <mergeCell ref="B63:H63"/>
-    <mergeCell ref="B64:H64"/>
-    <mergeCell ref="B65:H65"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="B67:H67"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="B54:H54"/>
-    <mergeCell ref="B55:H55"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B57:H57"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="B61:H61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1988,6 +2028,8 @@
     <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{45A35FFC-0B4A-493E-8BFD-51BF7BA22C92}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{54074182-9B44-45B7-97A7-8CCAD6B2DB90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Doc: Added Test Summary Report to CIL
</commit_message>
<xml_diff>
--- a/Project Management Plan/CIL.xlsx
+++ b/Project Management Plan/CIL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Project Management Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBF7B61-C6BA-43D8-8AFB-D7FAF69DA691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF287080-0B85-4A3A-BDB9-AE25F196D469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Item</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>Test Strategy Document</t>
+  </si>
+  <si>
+    <t>https://github.com/abdallahEl-Karamany/Online-Mobile-Store-WebSite/blob/339598636f84336db98477035e8e5461a70abc03/Test/Test-Summary-Report.docx</t>
+  </si>
+  <si>
+    <t>Test Summary Report</t>
+  </si>
+  <si>
+    <t>Online-Mobile-Store-WebSite/Test/Test-Summary-Report.docx</t>
   </si>
 </sst>
 </file>
@@ -335,19 +344,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -369,6 +368,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -590,8 +599,8 @@
   </sheetPr>
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:H19"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -607,37 +616,37 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="10" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -652,7 +661,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="22" t="s">
         <v>40</v>
       </c>
       <c r="J3" s="7"/>
@@ -662,26 +671,26 @@
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="19" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="7"/>
@@ -690,7 +699,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="22" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="7"/>
@@ -700,7 +709,7 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="7"/>
@@ -709,7 +718,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="22" t="s">
         <v>37</v>
       </c>
       <c r="J6" s="7"/>
@@ -719,26 +728,26 @@
       <c r="A7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="7"/>
@@ -747,7 +756,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="22" t="s">
         <v>36</v>
       </c>
       <c r="J8" s="7"/>
@@ -757,7 +766,7 @@
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="25" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7"/>
@@ -766,7 +775,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="22" t="s">
         <v>35</v>
       </c>
       <c r="J9" s="7"/>
@@ -776,7 +785,7 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="25" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="7"/>
@@ -785,7 +794,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="22" t="s">
         <v>34</v>
       </c>
       <c r="J10" s="7"/>
@@ -795,7 +804,7 @@
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="7"/>
@@ -804,7 +813,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="22" t="s">
         <v>33</v>
       </c>
       <c r="J11" s="7"/>
@@ -814,7 +823,7 @@
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="25" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="7"/>
@@ -823,7 +832,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="22" t="s">
         <v>32</v>
       </c>
       <c r="J12" s="7"/>
@@ -833,7 +842,7 @@
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="27" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="7"/>
@@ -852,7 +861,7 @@
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="7"/>
@@ -871,7 +880,7 @@
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="7"/>
@@ -890,7 +899,7 @@
       <c r="A16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="27" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="7"/>
@@ -909,7 +918,7 @@
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="27" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="7"/>
@@ -928,7 +937,7 @@
       <c r="A18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="27" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="7"/>
@@ -944,15 +953,21 @@
       <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="I19" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
@@ -1750,325 +1765,283 @@
       <c r="K80" s="7"/>
     </row>
     <row r="81" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="8"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
-      <c r="I81" s="8"/>
-      <c r="J81" s="8"/>
-      <c r="K81" s="8"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+      <c r="J81" s="24"/>
+      <c r="K81" s="24"/>
     </row>
     <row r="82" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="8"/>
-      <c r="J82" s="8"/>
-      <c r="K82" s="8"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="24"/>
+      <c r="H82" s="24"/>
+      <c r="I82" s="24"/>
+      <c r="J82" s="24"/>
+      <c r="K82" s="24"/>
     </row>
     <row r="83" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="8"/>
-      <c r="H83" s="8"/>
-      <c r="I83" s="8"/>
-      <c r="J83" s="8"/>
-      <c r="K83" s="8"/>
+      <c r="B83" s="24"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="24"/>
+      <c r="H83" s="24"/>
+      <c r="I83" s="24"/>
+      <c r="J83" s="24"/>
+      <c r="K83" s="24"/>
     </row>
     <row r="84" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
-      <c r="F84" s="8"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
-      <c r="I84" s="8"/>
-      <c r="J84" s="8"/>
-      <c r="K84" s="8"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="24"/>
+      <c r="K84" s="24"/>
     </row>
     <row r="85" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="8"/>
-      <c r="J85" s="8"/>
-      <c r="K85" s="8"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+      <c r="I85" s="24"/>
+      <c r="J85" s="24"/>
+      <c r="K85" s="24"/>
     </row>
     <row r="86" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="8"/>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="8"/>
-      <c r="J86" s="8"/>
-      <c r="K86" s="8"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="24"/>
+      <c r="J86" s="24"/>
+      <c r="K86" s="24"/>
     </row>
     <row r="87" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="8"/>
-      <c r="G87" s="8"/>
-      <c r="H87" s="8"/>
-      <c r="I87" s="8"/>
-      <c r="J87" s="8"/>
-      <c r="K87" s="8"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+      <c r="I87" s="24"/>
+      <c r="J87" s="24"/>
+      <c r="K87" s="24"/>
     </row>
     <row r="88" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="8"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8"/>
-      <c r="G88" s="8"/>
-      <c r="H88" s="8"/>
-      <c r="I88" s="8"/>
-      <c r="J88" s="8"/>
-      <c r="K88" s="8"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="24"/>
+      <c r="I88" s="24"/>
+      <c r="J88" s="24"/>
+      <c r="K88" s="24"/>
     </row>
     <row r="89" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="8"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
-      <c r="J89" s="8"/>
-      <c r="K89" s="8"/>
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
+      <c r="H89" s="24"/>
+      <c r="I89" s="24"/>
+      <c r="J89" s="24"/>
+      <c r="K89" s="24"/>
     </row>
     <row r="90" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="8"/>
-      <c r="H90" s="8"/>
-      <c r="I90" s="8"/>
-      <c r="J90" s="8"/>
-      <c r="K90" s="8"/>
+      <c r="B90" s="24"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="24"/>
+      <c r="H90" s="24"/>
+      <c r="I90" s="24"/>
+      <c r="J90" s="24"/>
+      <c r="K90" s="24"/>
     </row>
     <row r="91" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8"/>
-      <c r="J91" s="8"/>
-      <c r="K91" s="8"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
+      <c r="I91" s="24"/>
+      <c r="J91" s="24"/>
+      <c r="K91" s="24"/>
     </row>
     <row r="92" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="8"/>
-      <c r="K92" s="8"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="24"/>
+      <c r="J92" s="24"/>
+      <c r="K92" s="24"/>
     </row>
     <row r="93" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="8"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8"/>
-      <c r="J93" s="8"/>
-      <c r="K93" s="8"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+      <c r="I93" s="24"/>
+      <c r="J93" s="24"/>
+      <c r="K93" s="24"/>
     </row>
     <row r="94" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
-      <c r="J94" s="8"/>
-      <c r="K94" s="8"/>
+      <c r="B94" s="24"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="24"/>
+      <c r="H94" s="24"/>
+      <c r="I94" s="24"/>
+      <c r="J94" s="24"/>
+      <c r="K94" s="24"/>
     </row>
     <row r="95" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B95" s="8"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8"/>
-      <c r="K95" s="8"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="24"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
+      <c r="I95" s="24"/>
+      <c r="J95" s="24"/>
+      <c r="K95" s="24"/>
     </row>
     <row r="96" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="8"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
-      <c r="J96" s="8"/>
-      <c r="K96" s="8"/>
+      <c r="B96" s="24"/>
+      <c r="C96" s="24"/>
+      <c r="D96" s="24"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="24"/>
+      <c r="G96" s="24"/>
+      <c r="H96" s="24"/>
+      <c r="I96" s="24"/>
+      <c r="J96" s="24"/>
+      <c r="K96" s="24"/>
     </row>
     <row r="97" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B97" s="8"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="8"/>
-      <c r="H97" s="8"/>
-      <c r="I97" s="8"/>
-      <c r="J97" s="8"/>
-      <c r="K97" s="8"/>
+      <c r="B97" s="24"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="24"/>
+      <c r="I97" s="24"/>
+      <c r="J97" s="24"/>
+      <c r="K97" s="24"/>
     </row>
     <row r="98" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B98" s="8"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8"/>
-      <c r="I98" s="8"/>
-      <c r="J98" s="8"/>
-      <c r="K98" s="8"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="24"/>
+      <c r="I98" s="24"/>
+      <c r="J98" s="24"/>
+      <c r="K98" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="194">
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="I97:K97"/>
-    <mergeCell ref="I98:K98"/>
-    <mergeCell ref="I89:K89"/>
-    <mergeCell ref="I90:K90"/>
-    <mergeCell ref="I91:K91"/>
-    <mergeCell ref="I92:K92"/>
-    <mergeCell ref="I93:K93"/>
-    <mergeCell ref="I94:K94"/>
-    <mergeCell ref="I95:K95"/>
-    <mergeCell ref="I81:K81"/>
-    <mergeCell ref="I82:K82"/>
-    <mergeCell ref="I83:K83"/>
-    <mergeCell ref="I84:K84"/>
-    <mergeCell ref="I85:K85"/>
-    <mergeCell ref="I86:K86"/>
-    <mergeCell ref="I87:K87"/>
-    <mergeCell ref="I88:K88"/>
-    <mergeCell ref="I96:K96"/>
-    <mergeCell ref="I72:K72"/>
-    <mergeCell ref="I73:K73"/>
-    <mergeCell ref="I74:K74"/>
-    <mergeCell ref="I75:K75"/>
-    <mergeCell ref="I76:K76"/>
-    <mergeCell ref="I77:K77"/>
-    <mergeCell ref="I78:K78"/>
-    <mergeCell ref="I79:K79"/>
-    <mergeCell ref="I80:K80"/>
-    <mergeCell ref="I63:K63"/>
-    <mergeCell ref="I64:K64"/>
-    <mergeCell ref="I65:K65"/>
-    <mergeCell ref="I66:K66"/>
-    <mergeCell ref="I67:K67"/>
-    <mergeCell ref="I68:K68"/>
-    <mergeCell ref="I69:K69"/>
-    <mergeCell ref="I70:K70"/>
-    <mergeCell ref="I71:K71"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="I57:K57"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="I59:K59"/>
-    <mergeCell ref="I60:K60"/>
-    <mergeCell ref="I61:K61"/>
-    <mergeCell ref="I62:K62"/>
+    <mergeCell ref="B71:H71"/>
+    <mergeCell ref="B72:H72"/>
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="B82:H82"/>
+    <mergeCell ref="B83:H83"/>
+    <mergeCell ref="B73:H73"/>
+    <mergeCell ref="B74:H74"/>
+    <mergeCell ref="B75:H75"/>
+    <mergeCell ref="B76:H76"/>
+    <mergeCell ref="B77:H77"/>
+    <mergeCell ref="B78:H78"/>
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="B81:H81"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B64:H64"/>
+    <mergeCell ref="B65:H65"/>
+    <mergeCell ref="B66:H66"/>
+    <mergeCell ref="B67:H67"/>
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="B98:H98"/>
+    <mergeCell ref="B90:H90"/>
+    <mergeCell ref="B91:H91"/>
+    <mergeCell ref="B92:H92"/>
+    <mergeCell ref="B93:H93"/>
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B95:H95"/>
+    <mergeCell ref="B96:H96"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="B86:H86"/>
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="B88:H88"/>
+    <mergeCell ref="B89:H89"/>
+    <mergeCell ref="B97:H97"/>
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B50:H50"/>
     <mergeCell ref="B51:H51"/>
@@ -2093,6 +2066,65 @@
     <mergeCell ref="B45:H45"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B29:H29"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="I60:K60"/>
+    <mergeCell ref="I61:K61"/>
+    <mergeCell ref="I62:K62"/>
+    <mergeCell ref="I63:K63"/>
+    <mergeCell ref="I64:K64"/>
+    <mergeCell ref="I65:K65"/>
+    <mergeCell ref="I66:K66"/>
+    <mergeCell ref="I67:K67"/>
+    <mergeCell ref="I68:K68"/>
+    <mergeCell ref="I69:K69"/>
+    <mergeCell ref="I70:K70"/>
+    <mergeCell ref="I71:K71"/>
+    <mergeCell ref="I72:K72"/>
+    <mergeCell ref="I73:K73"/>
+    <mergeCell ref="I74:K74"/>
+    <mergeCell ref="I75:K75"/>
+    <mergeCell ref="I76:K76"/>
+    <mergeCell ref="I77:K77"/>
+    <mergeCell ref="I78:K78"/>
+    <mergeCell ref="I79:K79"/>
+    <mergeCell ref="I80:K80"/>
+    <mergeCell ref="I81:K81"/>
+    <mergeCell ref="I82:K82"/>
+    <mergeCell ref="I83:K83"/>
+    <mergeCell ref="I84:K84"/>
+    <mergeCell ref="I85:K85"/>
+    <mergeCell ref="I86:K86"/>
+    <mergeCell ref="I87:K87"/>
+    <mergeCell ref="I88:K88"/>
+    <mergeCell ref="I96:K96"/>
+    <mergeCell ref="I97:K97"/>
+    <mergeCell ref="I98:K98"/>
+    <mergeCell ref="I89:K89"/>
+    <mergeCell ref="I90:K90"/>
+    <mergeCell ref="I91:K91"/>
+    <mergeCell ref="I92:K92"/>
+    <mergeCell ref="I93:K93"/>
+    <mergeCell ref="I94:K94"/>
+    <mergeCell ref="I95:K95"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="B2:K2"/>
     <mergeCell ref="B30:H30"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="B32:H32"/>
@@ -2101,66 +2133,49 @@
     <mergeCell ref="B35:H35"/>
     <mergeCell ref="B36:H36"/>
     <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B98:H98"/>
-    <mergeCell ref="B90:H90"/>
-    <mergeCell ref="B91:H91"/>
-    <mergeCell ref="B92:H92"/>
-    <mergeCell ref="B93:H93"/>
-    <mergeCell ref="B94:H94"/>
-    <mergeCell ref="B95:H95"/>
-    <mergeCell ref="B96:H96"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B85:H85"/>
-    <mergeCell ref="B86:H86"/>
-    <mergeCell ref="B87:H87"/>
-    <mergeCell ref="B88:H88"/>
-    <mergeCell ref="B89:H89"/>
-    <mergeCell ref="B97:H97"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B82:H82"/>
-    <mergeCell ref="B83:H83"/>
-    <mergeCell ref="B73:H73"/>
-    <mergeCell ref="B74:H74"/>
-    <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B76:H76"/>
-    <mergeCell ref="B77:H77"/>
-    <mergeCell ref="B78:H78"/>
-    <mergeCell ref="B79:H79"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="B81:H81"/>
-    <mergeCell ref="B64:H64"/>
-    <mergeCell ref="B65:H65"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="B67:H67"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="B71:H71"/>
-    <mergeCell ref="B72:H72"/>
-    <mergeCell ref="B55:H55"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B57:H57"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="B62:H62"/>
-    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2180,6 +2195,7 @@
     <hyperlink ref="B16" r:id="rId15" xr:uid="{940A93D9-BBD4-4572-B914-62957599B52F}"/>
     <hyperlink ref="B17" r:id="rId16" xr:uid="{02C7378F-C901-4098-B6FE-CF0454F177F6}"/>
     <hyperlink ref="B18" r:id="rId17" xr:uid="{C7557FD7-E505-4E14-82EC-1D95BA317DD4}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{38877D7F-F692-44C0-956D-CE9A5A6F4BDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>